<commit_message>
Alteração de nomes e adição de skills
</commit_message>
<xml_diff>
--- a/Systems/IAron/Dev Assistant.xlsx
+++ b/Systems/IAron/Dev Assistant.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertn\Documents\Projetos\PYTHON\ppc-agent\Systems\IAron\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\robertn\Documents\Projetos\PYTHON\iaron-developer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F738203F-2ADB-4D88-8921-FA36E4166EB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A3E6FF3-8BBD-4432-9006-E900AB6DB6EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-45" windowWidth="29040" windowHeight="15840" xr2:uid="{D222F31E-51F6-45E8-9DE9-D5A867BE515D}"/>
+    <workbookView xWindow="6420" yWindow="630" windowWidth="21585" windowHeight="14640" xr2:uid="{D222F31E-51F6-45E8-9DE9-D5A867BE515D}"/>
   </bookViews>
   <sheets>
     <sheet name="Inteligencia" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="180">
   <si>
     <t>Objetivo</t>
   </si>
@@ -3298,11 +3298,41 @@
 percorrer toda a tabela, salvando em um dicionário os campos: "reqC","dataRem.","responsavel"</t>
   </si>
   <si>
+    <t>def COOIS():
+        select_transaction('COOIS')
+        insert_variant('MATERIAIS GTA')
+        run_actual_transaction()
+        my_grid = get_my_grid()
+        row_number = get_my_grid_count_rows(my_grid)
+        for i in range(row_number):
+            orders = f""{orders}{my_grid.getCellValue(i,'AUFNR')}\n"""</t>
+  </si>
+  <si>
+    <t>def ME5A():
+        select_transaction('ME5A')
+        insert_variant('WENLOG')
+        run_actual_transaction()
+        press_button('Selecionar layout...')
+        my_grid_select_layout('/WENLOG')
+        my_grid = get_my_grid()
+        rows = get_my_grid_count_rows(my_grid)
+        for i in range(rows):
+            reqs.append({'reqC':my_grid.getCellValue(i,'BANFN'), 'dataRem.':my_grid.getCellValue(i,'LFDAT'), 'responsavel':''"})</t>
+  </si>
+  <si>
     <t>Selecionar a transação ME52N no SAP
 pressionar o botão "Outra requisição de compra"
 escrever no campo "Requisição de compra" o texto "numeroTeste"
 Pressionar o botão "Outro documento"
 Se a janela atual do SAP for 1 então pressionar o botão "Não"</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    def ME52N(self, index:int):
+        select_transaction('ME52N')
+        press_button('Outra requisição de compra')
+        write_text_field('Requisição de compra',"numeroTeste")
+        press_button('Outro documento')
+        if session.activeWindow.name == 'wnd[1]':self.sap.press_button('Não')</t>
   </si>
   <si>
     <t>Título: Componentes Pendentes de Aprovação
@@ -5178,43 +5208,200 @@
                      work.copy)</t>
   </si>
   <si>
-    <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+    <t>Título: Python Default Script
+Descrição: Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+Solicitado por: Akira Ribeiral Okamoto
+Desenvolvido por: Robert Aron Zimmermann
+Observações:
+Adicionar Tratativas de erro para evitar que o código trave
+SAP deve estar com o idioma PT selecionado
+Procedimento:
+Abrir planilha "Materiais_1200.xlsx"
+Copiar todos os itens da coluna 1 quando o item da coluna 2 for igual a "MAT_BMRED_001" e o item da coluna 4 for igual a 1200
+Acessar transação ZTMM119
+Colar dados na seleção múltipla do campo "Material"
+No campo "Centro" escrever "1200"
+Executar Transação
+Clicar em "Listar características"
+Percorrer tabela atual
+Se o texto da coluna "ATBEZ" for igual a "COMPRIMENTO", "MATERIAL BARRA" ou "DIAMETRO EXTERNO" então flegar como True o Checkbox da coluna "XFELD"
+Clicar no botão session.findById("wnd[1]/tbar[0]/btn[3]")
+Escrever tabela na planilha Excel "Comparar.xlsx" aba Sem Necessidade
+Acessar CL30N
+No campo "Classe" escrever "MAT_BMRED_001"
+Escrever no campo "Tipo classe" o texto "001"
+Executar
+Fechar o documento word que aparecer
+Clicar em "Pesquisa na classe de acesso"
+Armazenar em uma variável os dados da coluna "OBJEK" da tabela
+Acessar transação ZTMM402
+Inserir variante "/WEN_APROVEITA"
+Colar os dados copiados no campo "Material"
+Executar
+Escrever tabela na planilha Excel "Comparar.xlsx" aba Com Necessidade</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model;
 import os
 import sys
-    def ME52N(self, index:int):
-        select_transaction('ME52N')
-        press_button('Outra requisição de compra')
-        write_text_field('Requisição de compra',""numeroTeste"")
-        press_button('Outro documento')
-        if session.activeWindow.name == 'wnd[1]':self.sap.press_button('Não')</t>
-  </si>
-  <si>
-    <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+from sap_functions import SAP
+from excel import ExcelHandler
+default_language = 'PT'
+login = open(f'{os.path.dirname(sys.argv[0])}\\sap_login.txt', 'r').readline().strip().split(',')
+scheduled_execution = {'scheduled?': False, 'username': login[0], 'password': login[1], 'principal': '100'}
+sap_window = 0
+# Python Default Script
+# Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+# Solicitado por Akira Ribeiral Okamoto
+# Desenvolvido por Robert Aron Zimmermann
+class Work:
+    def __init__(self):
+        self.sap = SAP(sap_window, scheduled_execution, default_language)
+        self.excel = ExcelHandler(f'{os.path.dirname(sys.argv[0])}\\Comparar.xlsx')
+        self.materials = []
+    def ZTMM119(self):
+        self.sap.select_transaction('ZTMM119')
+        self.sap.multiple_selection_field('Material')
+        self.sap.multiple_selection_paste_data('\n'.join(self.materials))
+        self.sap.write_text_field('Centro', '1200')
+        self.sap.run_actual_transaction()
+        self.sap.press_button('Listar características')
+        my_grid = self.sap.get_my_grid()
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        for i in range(rows):
+            if my_grid.getCellValue(i, 'ATBEZ') in ['COMPRIMENTO', 'MATERIAL BARRA', 'DIAMETRO EXTERNO']:
+                my_grid.modifyCheckbox(i, "XFELD", True)
+                my_grid.triggerModified()
+        self.sap.session.findById("wnd[1]/tbar[0]/btn[3]").press()
+        my_grid = self.sap.get_my_grid()
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        self.excel.load_workbook()
+        self.excel.select_sheet('Sem Necessidade')
+        self.excel.clean_data(2, self.excel.count_columns(1), 2, self.excel.count_rows(2))
+        self.excel.sap_write_my_grid(my_grid, rows, 1, 2)
+        self.excel.save_workbook()
+        self.excel.close_workbook()
+    def CL30N(self):
+        self.sap.select_transaction('CL30N')
+        self.sap.write_text_field('Classe', 'MAT_BMRED_001')
+        self.sap.write_text_field('Tipo classe', '001')
+        self.sap.run_actual_transaction()
+        self.sap.press_button('Fechar')
+        self.sap.press_button('Pesquisa na classe de acesso')
+        my_grid = self.sap.session.findById("wnd[0]/shellcont[1]/shell")
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        self.materials = []
+        for i in range(rows):
+            self.materials.append(my_grid.getCellValue(i, 'OBJEK'))
+    def ZTMM402(self):
+        self.sap.select_transaction('ZTMM402')
+        self.sap.insert_variant('/WEN_APROVEITA')
+        self.sap.multiple_selection_field('Material')
+        self.sap.multiple_selection_paste_data('\n'.join(self.materials))
+        self.sap.run_actual_transaction()
+        my_grid = self.sap.get_my_grid()
+        rows = self.sap.get_my_grid_count_rows(my_grid)
+        self.excel.load_workbook()
+        self.excel.select_sheet('Com Necessidade')
+        self.excel.clean_data(2, self.excel.count_columns(1), 2, self.excel.count_rows(2))
+        self.excel.sap_write_my_grid(my_grid, rows, 1, 2)
+        self.excel.save_workbook()
+        self.excel.close_workbook()
+if __name__ == '__main__':
+    work = Work()
+    excel = ExcelHandler(f'{os.path.dirname(sys.argv[0])}\\Materiais_1200.xlsx')
+    excel.load_workbook()
+    excel.select_sheet('Principal')
+    rows = excel.count_rows(1)
+    for i in range(2, rows + 1):
+        if excel.get_cell(i, 2) == 'MAT_BMRED_001' and excel.get_cell(i, 4) == 1200:
+            work.materials.append(str(excel.get_cell(i, 1)))
+    excel.close_workbook()
+    work.ZTMM119()
+    work.CL30N()
+    work.ZTMM402()
+</t>
+  </si>
+  <si>
+    <t>Título: Python Default Script
+Descrição: Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+Solicitado por: Akira Ribeiral Okamoto
+Desenvolvido por: Robert Aron Zimmermann
+Observações:
+Adicionar Tratativas de erro para evitar que o código trave
+SAP deve estar com o idioma PT selecionado
+Procedimento:
+Percorrer todas as linhas da planilha "Materiais_1200.xlsx"
+Para cada material da coluna 1:
+Acessar transação MM03
+Escrever no campo "Material" o valor do material
+Executar
+Clicar no botão "Avançar"
+Selecionar aba 2
+Clicar em Avançar
+Verificar se o texto da coluna "Denominação" do campo Flex não se encontra no arquivo "Exceções.txt"
+Caso não se encontre então armazenar o texto da coluna "Classe" do campo Flex  na coluna 2 na linha atual da planilha "Materiais_1200.xlsx"</t>
+  </si>
+  <si>
+    <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model;
 import os
 import sys
-    def ME5A():
-        select_transaction('ME5A')
-        insert_variant('WENLOG')
-        run_actual_transaction()
-        press_button('Selecionar layout...')
-        my_grid_select_layout('/WENLOG')
-        my_grid = get_my_grid()
-        rows = get_my_grid_count_rows(my_grid)
-        for i in range(rows):
-            reqs.append({'reqC':my_grid.getCellValue(i,'BANFN'), 'dataRem.':my_grid.getCellValue(i,'LFDAT'), 'responsavel':''"})</t>
-  </si>
-  <si>
-    <t># Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
-import os
-import sys
-    def COOIS():
-        select_transaction('COOIS')
-        insert_variant('MATERIAIS GTA')
-        run_actual_transaction()
-        my_grid = get_my_grid()
-        row_number = get_my_grid_count_rows(my_grid)
-        for i in range(row_number):
-            orders = f""{orders}{my_grid.getCellValue(i,'AUFNR')}\n"""</t>
+from sap_functions import SAP
+from excel import ExcelHandler
+default_language = 'PT'
+login = open(f'{os.path.dirname(sys.argv[0])}\\sap_login.txt', 'r').readline().strip().split(',')
+scheduled_execution = {'scheduled?': False, 'username': login[0], 'password': login[1], 'principal': '100'}
+sap_window = 0
+# Python Default Script
+# Default model for SAP automations, developed by Robert Aron Zimmermann, using Google AI Studio tuned prompt model
+# Solicitado por: Akira Ribeiral Okamoto
+# Desenvolvido por: Robert Aron Zimmermann
+class Work:
+    def __init__(self):
+        self.sap = SAP(sap_window, scheduled_execution, default_language)
+        self.excel = ExcelHandler(f'{os.path.dirname(sys.argv[0])}\\Materiais_1200.xlsx')
+    def MM03(self, material):
+        self.sap.select_transaction('MM03')
+        self.sap.write_text_field('Material', material)
+        self.sap.run_actual_transaction()
+        self.sap.press_button('Avançar')
+        self.sap.change_active_tab(2)
+        if self.sap.session.activeWindow.name == 'wnd[1]':
+            self.sap.press_button('Avançar', selected_tab=2)
+        total_linhas = int(self.sap.session.findById("wnd[0]/usr/txtRMCLF-PAGANZ").text)
+        while int(self.sap.session.findById("wnd[0]/usr/txtRMCLF-PAGPOS").text) &lt;= total_linhas:
+            my_table = self.sap.get_my_table()
+            classe = my_table.getCell(0, 0).Text
+            exception = False
+            with open(f'{os.path.dirname(sys.argv[0])}\\Exceções.txt', 'r') as file:
+                for line in file:
+                    if classe == line.strip():
+                        exception = True
+            if not exception:
+                print(f'Escreveu {classe} no material {material}')
+                self.excel.write_cell(row, 2, classe)
+                return
+            if exception and int(self.sap.session.findById("wnd[0]/usr/txtRMCLF-PAGPOS").text) == total_linhas:
+                return
+            self.sap.session.findById("wnd[0]/usr/txtRMCLF-PAGPOS").text = int(self.sap.session.findById("wnd[0]/usr/txtRMCLF-PAGPOS").text) + 1
+            self.sap.session.findById('wnd[0]').sendVKey(0)
+if __name__ == '__main__':
+    work = Work()
+    work.excel.load_workbook()
+    work.excel.select_sheet('Principal')
+    rows = work.excel.count_rows(1)
+    for row in range(2, rows + 1):
+        material = work.excel.get_cell(row, 1)
+        if material is not None:
+            try:
+                if work.excel.get_cell(row, 2) is None:
+                    work.MM03(material)
+                    work.excel.save_workbook()
+            except Exception as e:
+                work.excel.write_cell(row, 2, f'Ocorreu o erro: {e}')
+            finally:
+                work.excel.close_workbook()
+    work.excel.close_workbook()</t>
   </si>
 </sst>
 </file>
@@ -5617,10 +5804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AA211B0-CF30-4FF4-82D8-F1F44D488D73}">
-  <dimension ref="A1:B90"/>
+  <dimension ref="A1:B92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A68" workbookViewId="0">
-      <selection activeCell="B71" sqref="B71"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="A93" sqref="A93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6186,7 +6373,7 @@
         <v>134</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>175</v>
+        <v>136</v>
       </c>
     </row>
     <row r="71" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6194,159 +6381,175 @@
         <v>135</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>174</v>
+        <v>137</v>
       </c>
     </row>
     <row r="72" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>173</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
     </row>
     <row r="74" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
     </row>
     <row r="76" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
     </row>
     <row r="78" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="79" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
     </row>
     <row r="80" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
     </row>
     <row r="81" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
     </row>
     <row r="82" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
     </row>
     <row r="84" spans="1:2" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
-        <v>149</v>
+        <v>152</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
     </row>
     <row r="85" spans="1:2" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="86" spans="1:2" ht="130.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
     </row>
     <row r="87" spans="1:2" ht="91.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
     </row>
     <row r="88" spans="1:2" ht="166.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
     </row>
     <row r="89" spans="1:2" ht="218.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
     </row>
     <row r="90" spans="1:2" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>156</v>
+        <v>159</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="B91" s="2" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" ht="152.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B92" s="2" t="s">
+        <v>179</v>
       </c>
     </row>
   </sheetData>

</xml_diff>